<commit_message>
on semi link updated
</commit_message>
<xml_diff>
--- a/data/Semiconductor_Companies_Careers_Updated.xlsx
+++ b/data/Semiconductor_Companies_Careers_Updated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham09\Downloads\git repo\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham09\Downloads\job-search-agent\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3D135E-9DDC-49F8-B6AC-46183ED19547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246BC5BF-8FFB-40E3-A045-D8863ECD1808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semiconductor Companies" sheetId="1" r:id="rId1"/>
@@ -153,9 +153,6 @@
     <t>Onsemi</t>
   </si>
   <si>
-    <t>https://www.onsemi.com/careers</t>
-  </si>
-  <si>
     <t>Skyworks Solutions</t>
   </si>
   <si>
@@ -523,6 +520,9 @@
   </si>
   <si>
     <t>https://sec.wd3.myworkdayjobs.com/Samsung_Careers</t>
+  </si>
+  <si>
+    <t>https://hctz.fa.us2.oraclecloud.com/hcmUI/CandidateExperience/en/sites/CX_1001/jobs?mode=location</t>
   </si>
 </sst>
 </file>
@@ -968,8 +968,8 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1239,8 +1239,8 @@
       <c r="B19" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>41</v>
+      <c r="C19" s="17" t="s">
+        <v>164</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>6</v>
@@ -1251,10 +1251,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>6</v>
@@ -1265,10 +1265,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>6</v>
@@ -1279,10 +1279,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>6</v>
@@ -1293,10 +1293,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>49</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>6</v>
@@ -1307,10 +1307,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>6</v>
@@ -1321,10 +1321,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>52</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>53</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>6</v>
@@ -1335,10 +1335,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>6</v>
@@ -1349,10 +1349,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>6</v>
@@ -1363,10 +1363,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>6</v>
@@ -1377,10 +1377,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>60</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>61</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>6</v>
@@ -1391,10 +1391,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="14" t="s">
         <v>62</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>63</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>6</v>
@@ -1405,10 +1405,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>6</v>
@@ -1419,10 +1419,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>6</v>
@@ -1433,10 +1433,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>69</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>6</v>
@@ -1447,10 +1447,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>6</v>
@@ -1461,10 +1461,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="15" t="s">
         <v>72</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>73</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>6</v>
@@ -1475,10 +1475,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>6</v>
@@ -1489,10 +1489,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>77</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>6</v>
@@ -1503,10 +1503,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="14" t="s">
         <v>78</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>79</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>6</v>
@@ -1517,10 +1517,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>80</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>81</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>6</v>
@@ -1531,10 +1531,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="14" t="s">
         <v>82</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>83</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>6</v>
@@ -1545,10 +1545,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>6</v>
@@ -1559,10 +1559,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="14" t="s">
         <v>86</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>87</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>6</v>
@@ -1573,10 +1573,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>89</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>6</v>
@@ -1587,10 +1587,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>6</v>
@@ -1601,10 +1601,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>93</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>6</v>
@@ -1615,10 +1615,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="14" t="s">
         <v>94</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>95</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>6</v>
@@ -1629,10 +1629,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>96</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>6</v>
@@ -1643,10 +1643,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="14" t="s">
         <v>98</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>99</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>6</v>
@@ -1657,10 +1657,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>100</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>101</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>6</v>
@@ -1671,10 +1671,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>6</v>
@@ -1685,10 +1685,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>6</v>
@@ -1699,10 +1699,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="14" t="s">
         <v>106</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>107</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>6</v>
@@ -1713,10 +1713,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>6</v>
@@ -1727,10 +1727,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>6</v>
@@ -1741,10 +1741,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="15" t="s">
         <v>112</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>113</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>6</v>
@@ -1755,10 +1755,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>6</v>
@@ -1769,10 +1769,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>117</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>6</v>
@@ -1783,10 +1783,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>119</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>6</v>
@@ -1797,10 +1797,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>121</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>6</v>
@@ -1811,10 +1811,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>6</v>
@@ -1825,13 +1825,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D61" s="13" t="s">
         <v>124</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="D61" s="13" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1839,13 +1839,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C62" s="12" t="s">
-        <v>127</v>
-      </c>
       <c r="D62" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1853,13 +1853,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="C63" s="16" t="s">
-        <v>129</v>
-      </c>
       <c r="D63" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1867,13 +1867,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="C64" s="16" t="s">
-        <v>131</v>
-      </c>
       <c r="D64" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1881,13 +1881,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C65" s="12" t="s">
-        <v>133</v>
-      </c>
       <c r="D65" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1895,13 +1895,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C66" s="12" t="s">
-        <v>135</v>
-      </c>
       <c r="D66" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1909,13 +1909,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C67" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="C67" s="16" t="s">
-        <v>137</v>
-      </c>
       <c r="D67" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1923,13 +1923,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="12" t="s">
-        <v>139</v>
-      </c>
       <c r="D68" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1937,13 +1937,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C69" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C69" s="12" t="s">
-        <v>141</v>
-      </c>
       <c r="D69" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1951,13 +1951,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C70" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C70" s="12" t="s">
-        <v>143</v>
-      </c>
       <c r="D70" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1965,13 +1965,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C71" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="C71" s="16" t="s">
-        <v>145</v>
-      </c>
       <c r="D71" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1979,13 +1979,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C72" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="C72" s="16" t="s">
-        <v>147</v>
-      </c>
       <c r="D72" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1993,13 +1993,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C73" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C73" s="16" t="s">
-        <v>149</v>
-      </c>
       <c r="D73" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -2007,13 +2007,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C74" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="C74" s="12" t="s">
-        <v>151</v>
-      </c>
       <c r="D74" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -2021,13 +2021,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C75" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="C75" s="16" t="s">
-        <v>153</v>
-      </c>
       <c r="D75" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -2035,13 +2035,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C76" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="C76" s="16" t="s">
-        <v>155</v>
-      </c>
       <c r="D76" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -2049,13 +2049,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C77" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C77" s="16" t="s">
-        <v>157</v>
-      </c>
       <c r="D77" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -2063,10 +2063,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>157</v>
+      </c>
+      <c r="C78" t="s">
         <v>158</v>
-      </c>
-      <c r="C78" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -2074,10 +2074,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>159</v>
+      </c>
+      <c r="C79" t="s">
         <v>160</v>
-      </c>
-      <c r="C79" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -2085,10 +2085,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>161</v>
+      </c>
+      <c r="C80" t="s">
         <v>162</v>
-      </c>
-      <c r="C80" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semi companies links update
</commit_message>
<xml_diff>
--- a/data/Semiconductor_Companies_Careers_Updated.xlsx
+++ b/data/Semiconductor_Companies_Careers_Updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham09\Downloads\job-search-agent\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246BC5BF-8FFB-40E3-A045-D8863ECD1808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E93FA99-96A8-4DD2-B71E-C4782CE4A987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,30 +147,18 @@
     <t>Wolfspeed</t>
   </si>
   <si>
-    <t>https://www.wolfspeed.com/careers/</t>
-  </si>
-  <si>
     <t>Onsemi</t>
   </si>
   <si>
     <t>Skyworks Solutions</t>
   </si>
   <si>
-    <t>https://careers.skyworksinc.com/</t>
-  </si>
-  <si>
     <t>GlobalFoundries</t>
   </si>
   <si>
-    <t>https://gf.com/careers/</t>
-  </si>
-  <si>
     <t>Synopsys</t>
   </si>
   <si>
-    <t>https://careers.synopsys.com/</t>
-  </si>
-  <si>
     <t>Cadence Design Systems</t>
   </si>
   <si>
@@ -198,15 +186,9 @@
     <t>Tokyo Electron (TEL) US</t>
   </si>
   <si>
-    <t>https://www.tel.com/careers/</t>
-  </si>
-  <si>
     <t>Entegris</t>
   </si>
   <si>
-    <t>https://www.entegris.com/careers</t>
-  </si>
-  <si>
     <t>Advantest America</t>
   </si>
   <si>
@@ -222,27 +204,15 @@
     <t>Infineon Technologies</t>
   </si>
   <si>
-    <t>https://www.infineon.com/careers</t>
-  </si>
-  <si>
     <t>Polar Semiconductor</t>
   </si>
   <si>
-    <t>https://polarsemi.com/careers/</t>
-  </si>
-  <si>
     <t>Allegro MicroSystems</t>
   </si>
   <si>
-    <t>https://www.allegromicro.com/en/about-allegro/careers</t>
-  </si>
-  <si>
     <t>FormFactor</t>
   </si>
   <si>
-    <t>https://www.formfactor.com/company/careers/</t>
-  </si>
-  <si>
     <t>Coherent Corp</t>
   </si>
   <si>
@@ -252,15 +222,9 @@
     <t>MKS Instruments</t>
   </si>
   <si>
-    <t>https://www.mksinst.com/careers</t>
-  </si>
-  <si>
     <t>Brooks Automation</t>
   </si>
   <si>
-    <t>https://www.brooks.com/careers/</t>
-  </si>
-  <si>
     <t>Cohu</t>
   </si>
   <si>
@@ -294,9 +258,6 @@
     <t>Axcelis Technologies</t>
   </si>
   <si>
-    <t>https://www.axcelis.com/careers/</t>
-  </si>
-  <si>
     <t>Amkor Technology</t>
   </si>
   <si>
@@ -306,9 +267,6 @@
     <t>Kulicke &amp; Soffa (K&amp;S)</t>
   </si>
   <si>
-    <t>https://www.kns.com/Careers/Careers/Grow-with-K-S</t>
-  </si>
-  <si>
     <t>Veeco Instruments</t>
   </si>
   <si>
@@ -318,9 +276,6 @@
     <t>Onto Innovation</t>
   </si>
   <si>
-    <t>https://www.ontoinnovation.com/careers</t>
-  </si>
-  <si>
     <t>Formic</t>
   </si>
   <si>
@@ -330,21 +285,12 @@
     <t>Tenstorrent</t>
   </si>
   <si>
-    <t>https://tenstorrent.com/en/careers</t>
-  </si>
-  <si>
     <t>Rambus</t>
   </si>
   <si>
-    <t>https://careers.rambus.com/</t>
-  </si>
-  <si>
     <t>Cirrus Logic</t>
   </si>
   <si>
-    <t>https://www.cirrus.com/careers</t>
-  </si>
-  <si>
     <t>Monolithic Power Systems (MPS)</t>
   </si>
   <si>
@@ -390,9 +336,6 @@
     <t>Moog Inc.</t>
   </si>
   <si>
-    <t>https://www.moog.com/careers.html</t>
-  </si>
-  <si>
     <t>Harmonic Drive LLC</t>
   </si>
   <si>
@@ -408,9 +351,6 @@
     <t>Qorvo</t>
   </si>
   <si>
-    <t>https://careers.qorvo.com/</t>
-  </si>
-  <si>
     <t>SK Hynix America</t>
   </si>
   <si>
@@ -426,15 +366,9 @@
     <t>Silicon Labs</t>
   </si>
   <si>
-    <t>https://www.silabs.com/about-us/careers</t>
-  </si>
-  <si>
     <t>SkyWater Technology</t>
   </si>
   <si>
-    <t>https://www.skywatertechnology.com/careers/</t>
-  </si>
-  <si>
     <t>Ampere Computing</t>
   </si>
   <si>
@@ -444,21 +378,12 @@
     <t>Cerebras Systems</t>
   </si>
   <si>
-    <t>https://www.cerebras.ai/open-positions</t>
-  </si>
-  <si>
     <t>MACOM Technology</t>
   </si>
   <si>
-    <t>https://www.macom.com/about-macom/careers</t>
-  </si>
-  <si>
     <t>Lumentum</t>
   </si>
   <si>
-    <t>https://www.lumentum.com/en/careers</t>
-  </si>
-  <si>
     <t>Vishay Intertechnology</t>
   </si>
   <si>
@@ -523,6 +448,81 @@
   </si>
   <si>
     <t>https://hctz.fa.us2.oraclecloud.com/hcmUI/CandidateExperience/en/sites/CX_1001/jobs?mode=location</t>
+  </si>
+  <si>
+    <t>https://cree.wd108.myworkdayjobs.com/EXT</t>
+  </si>
+  <si>
+    <t>https://careers.skyworksinc.com/go/Information-Technology-Careers-At-Skyworks/2248300/</t>
+  </si>
+  <si>
+    <t>https://globalfoundries.wd1.myworkdayjobs.com/External</t>
+  </si>
+  <si>
+    <t>https://careers.synopsys.com/search-jobs</t>
+  </si>
+  <si>
+    <t>https://tel.wd3.myworkdayjobs.com/en-US/TEL-Careers</t>
+  </si>
+  <si>
+    <t>https://entegris.wd1.myworkdayjobs.com/EntegrisCareers</t>
+  </si>
+  <si>
+    <t>https://jobs.infineon.com/careers/</t>
+  </si>
+  <si>
+    <t>https://polarsemi.wd501.myworkdayjobs.com/Polar</t>
+  </si>
+  <si>
+    <t>https://allegromicro.wd5.myworkdayjobs.com/AllegroCareers</t>
+  </si>
+  <si>
+    <t>https://formfactor.wd1.myworkdayjobs.com/FFI-Careers</t>
+  </si>
+  <si>
+    <t>https://mksinst.wd1.myworkdayjobs.com/MKSCareersAmericas</t>
+  </si>
+  <si>
+    <t>https://brooksauto.wd1.myworkdayjobs.com/en-US/Brooks_External_Site</t>
+  </si>
+  <si>
+    <t>https://axcelis.wd1.myworkdayjobs.com/axcelis</t>
+  </si>
+  <si>
+    <t>https://etyy.fa.ap2.oraclecloud.com/hcmUI/CandidateExperience/en/sites/CX_1/jobs</t>
+  </si>
+  <si>
+    <t>https://wd1.myworkdaysite.com/recruiting/onto/ONTO_Careers</t>
+  </si>
+  <si>
+    <t>https://job-boards.greenhouse.io/tenstorrent</t>
+  </si>
+  <si>
+    <t>https://careers-rambus.icims.com/jobs/search</t>
+  </si>
+  <si>
+    <t>https://jobs.eu.lever.co/cirrus</t>
+  </si>
+  <si>
+    <t>https://silabs.wd1.myworkdayjobs.com/SiliconLabsCareers</t>
+  </si>
+  <si>
+    <t>https://jobs.dayforcehcm.com/en-US/skywater/CANDIDATEPORTAL</t>
+  </si>
+  <si>
+    <t>https://job-boards.greenhouse.io/cerebrassystems</t>
+  </si>
+  <si>
+    <t>https://macomtech.csod.com/ux/ats/careersite/4/home?c=macomtech</t>
+  </si>
+  <si>
+    <t>https://lumentum.wd5.myworkdayjobs.com/LITE</t>
+  </si>
+  <si>
+    <t>https://careers.qorvo.com/search/</t>
+  </si>
+  <si>
+    <t>https://moog.wd5.myworkdayjobs.com/MOOG_External_Career_Site</t>
   </si>
 </sst>
 </file>
@@ -968,8 +968,8 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1225,8 +1225,8 @@
       <c r="B18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>39</v>
+      <c r="C18" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>6</v>
@@ -1237,10 +1237,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>6</v>
@@ -1251,10 +1251,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>6</v>
@@ -1265,10 +1265,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>142</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>6</v>
@@ -1279,10 +1279,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>143</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>6</v>
@@ -1293,10 +1293,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>6</v>
@@ -1307,10 +1307,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>6</v>
@@ -1321,10 +1321,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>6</v>
@@ -1335,10 +1335,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>6</v>
@@ -1349,10 +1349,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>6</v>
@@ -1363,10 +1363,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>145</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>6</v>
@@ -1377,10 +1377,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>6</v>
@@ -1391,10 +1391,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>6</v>
@@ -1405,10 +1405,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>146</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>6</v>
@@ -1419,10 +1419,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>66</v>
+        <v>58</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>147</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>6</v>
@@ -1433,10 +1433,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>68</v>
+        <v>59</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>148</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>6</v>
@@ -1447,10 +1447,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>70</v>
+        <v>60</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>149</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>6</v>
@@ -1461,10 +1461,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>6</v>
@@ -1475,10 +1475,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>74</v>
+        <v>63</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>150</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>6</v>
@@ -1489,10 +1489,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>76</v>
+        <v>64</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>151</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>6</v>
@@ -1503,10 +1503,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>6</v>
@@ -1517,10 +1517,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>6</v>
@@ -1531,10 +1531,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>6</v>
@@ -1545,10 +1545,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>6</v>
@@ -1559,10 +1559,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>6</v>
@@ -1573,10 +1573,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>88</v>
+        <v>75</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>152</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>6</v>
@@ -1587,10 +1587,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>6</v>
@@ -1601,10 +1601,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>92</v>
+        <v>78</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>153</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>6</v>
@@ -1615,10 +1615,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>6</v>
@@ -1629,10 +1629,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>96</v>
+        <v>81</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>154</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>6</v>
@@ -1643,10 +1643,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>6</v>
@@ -1657,10 +1657,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>100</v>
+        <v>84</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>155</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>6</v>
@@ -1671,10 +1671,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>102</v>
+        <v>85</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>156</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>6</v>
@@ -1685,10 +1685,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>104</v>
+        <v>86</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>157</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>6</v>
@@ -1699,10 +1699,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>6</v>
@@ -1713,10 +1713,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>6</v>
@@ -1727,10 +1727,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>6</v>
@@ -1741,10 +1741,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>6</v>
@@ -1755,10 +1755,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>6</v>
@@ -1769,10 +1769,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>6</v>
@@ -1783,10 +1783,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>6</v>
@@ -1797,10 +1797,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>120</v>
+        <v>101</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>164</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>6</v>
@@ -1811,10 +1811,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>6</v>
@@ -1825,13 +1825,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1839,13 +1839,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>126</v>
+        <v>106</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>163</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1853,13 +1853,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1867,13 +1867,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1881,13 +1881,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>132</v>
+        <v>111</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>158</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1895,13 +1895,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>134</v>
+        <v>112</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>159</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1909,13 +1909,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1923,13 +1923,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>138</v>
+        <v>115</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>160</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1937,13 +1937,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C69" s="12" t="s">
-        <v>140</v>
+        <v>116</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>161</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1951,13 +1951,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>142</v>
+        <v>117</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>162</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1965,13 +1965,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1979,13 +1979,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="D72" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1993,13 +1993,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -2007,13 +2007,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -2021,13 +2021,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -2035,13 +2035,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -2049,13 +2049,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -2063,10 +2063,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>157</v>
-      </c>
-      <c r="C78" t="s">
-        <v>158</v>
+        <v>132</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -2074,10 +2074,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>159</v>
-      </c>
-      <c r="C79" t="s">
-        <v>160</v>
+        <v>134</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -2085,10 +2085,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>161</v>
-      </c>
-      <c r="C80" t="s">
-        <v>162</v>
+        <v>136</v>
+      </c>
+      <c r="C80" s="17" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2170,6 +2170,9 @@
     <hyperlink ref="C75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
     <hyperlink ref="C76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
     <hyperlink ref="C77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="C78" r:id="rId77" xr:uid="{B1077543-EE7F-4813-B1F7-653E6DFCC5D2}"/>
+    <hyperlink ref="C79" r:id="rId78" xr:uid="{0C06CABB-76D2-4514-9931-94F5C7983162}"/>
+    <hyperlink ref="C80" r:id="rId79" xr:uid="{F4B52E48-1FA2-496F-9B6C-80C7C617A444}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>